<commit_message>
Duplication prevention and Upload to service
</commit_message>
<xml_diff>
--- a/Web/UserEx.Web/wwwroot/Files/DIDs.xlsx
+++ b/Web/UserEx.Web/wwwroot/Files/DIDs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emil.hristov\OneDrive - Tiebreak Solutions\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://naxex-my.sharepoint.com/personal/emil_hristov_tiebreak_solutions/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F530BF2-4604-45EB-A63E-605AA329FB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{4F530BF2-4604-45EB-A63E-605AA329FB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1461042-E4AA-4AA9-BE6F-7659B31ECD95}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -393,7 +393,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,7 +447,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>448455642104</v>
+        <v>448455642999</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
@@ -592,7 +592,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>448455642109</v>
+        <v>448455642998</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>

</xml_diff>